<commit_message>
Respond to PIXm comments
</commit_message>
<xml_diff>
--- a/FHIR-R4/ITI_Comment_Form-PIXm_Felhofer.xlsx
+++ b/FHIR-R4/ITI_Comment_Form-PIXm_Felhofer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john.moehrke\Git\IT-Infrastructure\FHIR-R4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243E2506-12DB-4927-821C-07E496434175}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951C3180-DE75-4169-A35E-B93211E4C071}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="113">
   <si>
     <t>Priority</t>
   </si>
@@ -627,13 +627,52 @@
 Appendix E.3 is not in Vol 2x. I looked in a few other Supplements to no avail.   Was it supposed to be added by this supplement with FHIR details, or is the reference wrong?</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
     <t>Response</t>
+  </si>
+  <si>
+    <t>presume PRIM is close enough</t>
+  </si>
+  <si>
+    <t>discuss</t>
+  </si>
+  <si>
+    <t>Done
+No Change</t>
+  </si>
+  <si>
+    <t>No Change</t>
+  </si>
+  <si>
+    <t>I would prefer to not force grouping. I don't see a functional reason in PIXm that time needs to be any more accurate than not. There is no clock in the interface. If someone includes audit logging, then they will bring it in for that purpose. Forced groups tend to be fragile (see ATNA TLS problem), where as failure to group can result in idiots doing stupid stuff.
+No clear why we would need a note to indicate that this is intentionally different than PIX (especially since PIX likely should not have included it).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am not sure if the PRIM Feed should be brought into here. I think it is good only existing in PRIM. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">done </t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leave only FHIR </t>
+  </si>
+  <si>
+    <t>agree that it is unclear what the sentence was trying to convey that was not already said better.</t>
+  </si>
+  <si>
+    <t>specifically true, but what alternative is better? This seems the best value, and we do clarify the reason in the OperationOutcome
+Possibly we could use 404 for both leaving OperationOutcome to differentiate?</t>
+  </si>
+  <si>
+    <t>I think the restructuring helped clarify?</t>
+  </si>
+  <si>
+    <t>Appendix E updates are in our Appendix Z supplement (last page).</t>
   </si>
 </sst>
 </file>
@@ -849,7 +888,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -934,17 +973,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1285,8 +1343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,42 +1356,43 @@
     <col min="6" max="6" width="44" customWidth="1"/>
     <col min="7" max="7" width="49.7109375" style="20" customWidth="1"/>
     <col min="8" max="8" width="7.7109375" style="14" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="35" customWidth="1"/>
+    <col min="10" max="10" width="78" style="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
     </row>
     <row r="2" spans="1:10" ht="269.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
     </row>
     <row r="3" spans="1:10" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:10" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I4" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="J4" s="36"/>
+      <c r="I4" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -1360,11 +1419,11 @@
       <c r="H5" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="34" t="s">
+      <c r="I5" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="J5" s="32" t="s">
         <v>98</v>
-      </c>
-      <c r="J5" s="34" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
@@ -1392,8 +1451,14 @@
       <c r="H6" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" s="9" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+      <c r="I6" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="J6" s="41" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>63</v>
       </c>
@@ -1417,6 +1482,12 @@
       </c>
       <c r="H7" s="7" t="s">
         <v>9</v>
+      </c>
+      <c r="I7" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="J7" s="41" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
@@ -1442,6 +1513,12 @@
       <c r="H8" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="I8" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="J8" s="41" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="9" spans="1:10" s="9" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -1468,6 +1545,10 @@
       <c r="H9" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="I9" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="J9" s="41"/>
     </row>
     <row r="10" spans="1:10" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -1494,6 +1575,12 @@
       <c r="H10" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="I10" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="J10" s="41" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="11" spans="1:10" s="9" customFormat="1" ht="39" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -1520,6 +1607,10 @@
       <c r="H11" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="I11" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="J11" s="41"/>
     </row>
     <row r="12" spans="1:10" s="9" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -1546,6 +1637,12 @@
       <c r="H12" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="I12" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="J12" s="41" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="13" spans="1:10" s="9" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -1572,8 +1669,12 @@
       <c r="H13" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="I13" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="J13" s="41"/>
+    </row>
+    <row r="14" spans="1:10" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -1596,6 +1697,12 @@
       <c r="H14" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="I14" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="J14" s="41" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="15" spans="1:10" s="9" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
@@ -1622,6 +1729,12 @@
       <c r="H15" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="I15" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="J15" s="41" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="16" spans="1:10" s="9" customFormat="1" ht="39" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
@@ -1648,8 +1761,12 @@
       <c r="H16" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="I16" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="J16" s="41"/>
+    </row>
+    <row r="17" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>63</v>
       </c>
@@ -1674,8 +1791,12 @@
       <c r="H17" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="I17" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="J17" s="41"/>
+    </row>
+    <row r="18" spans="1:10" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>63</v>
       </c>
@@ -1700,8 +1821,14 @@
       <c r="H18" s="22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="J18" s="39" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="31"/>
       <c r="C19" s="8"/>
@@ -1711,7 +1838,7 @@
       <c r="G19" s="21"/>
       <c r="H19" s="17"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="31"/>
       <c r="C20" s="8"/>
@@ -1721,7 +1848,7 @@
       <c r="G20" s="21"/>
       <c r="H20" s="17"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="31"/>
       <c r="C21" s="8"/>
@@ -1731,7 +1858,7 @@
       <c r="G21" s="21"/>
       <c r="H21" s="17"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="31"/>
       <c r="C22" s="1"/>
@@ -1741,7 +1868,7 @@
       <c r="G22" s="21"/>
       <c r="H22" s="17"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="31"/>
       <c r="C23" s="1"/>
@@ -1751,7 +1878,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="17"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="31"/>
       <c r="C24" s="1"/>
@@ -1761,7 +1888,7 @@
       <c r="G24" s="16"/>
       <c r="H24" s="17"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="31"/>
       <c r="C25" s="1"/>
@@ -1771,7 +1898,7 @@
       <c r="G25" s="16"/>
       <c r="H25" s="17"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="31"/>
       <c r="C26" s="1"/>
@@ -1781,7 +1908,7 @@
       <c r="G26" s="16"/>
       <c r="H26" s="17"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="31"/>
       <c r="C27" s="1"/>
@@ -1791,7 +1918,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="17"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="31"/>
       <c r="C28" s="1"/>
@@ -1801,7 +1928,7 @@
       <c r="G28" s="5"/>
       <c r="H28" s="17"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="31"/>
       <c r="C29" s="1"/>
@@ -1811,7 +1938,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="17"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="31"/>
       <c r="C30" s="1"/>
@@ -1821,7 +1948,7 @@
       <c r="G30" s="22"/>
       <c r="H30" s="17"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="31"/>
       <c r="C31" s="1"/>
@@ -1831,7 +1958,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="17"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="31"/>
       <c r="C32" s="1"/>

</xml_diff>